<commit_message>
added last part of traceabilityMat and added class dropPoint to class diagram
</commit_message>
<xml_diff>
--- a/TraceabilityMatrix.xlsx
+++ b/TraceabilityMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Fabio\Documents\Polito\Software Engineering\Project\EzWh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969C7FAD-50E5-4380-9849-F4FBDB9A4E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB03875-F853-4D85-B1C9-8B212B4417A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="8100" xr2:uid="{80723916-DD60-4B65-A331-69E56BD6B192}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="143">
   <si>
     <t>FR1</t>
   </si>
@@ -437,6 +437,33 @@
   </si>
   <si>
     <t>IssueRestockOrder</t>
+  </si>
+  <si>
+    <t>CommitReturnOrder</t>
+  </si>
+  <si>
+    <t>ReturnOrder</t>
+  </si>
+  <si>
+    <t>createNewInternalOrders</t>
+  </si>
+  <si>
+    <t>deleteInternalOrders</t>
+  </si>
+  <si>
+    <t>modifyInternalOrders</t>
+  </si>
+  <si>
+    <t>IssueInternalOrder</t>
+  </si>
+  <si>
+    <t>DropPoint</t>
+  </si>
+  <si>
+    <t>ModifyDropPointOfInternalOrder</t>
+  </si>
+  <si>
+    <t>DeleteItemFromInternalOrder</t>
   </si>
 </sst>
 </file>
@@ -805,11 +832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0587820B-A026-4E1A-BA20-2653106DB9B3}">
-  <dimension ref="A1:BC80"/>
+  <dimension ref="A1:BC89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB77" sqref="AB77"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB82" sqref="BB82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,6 +1157,9 @@
       <c r="AJ14" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="BB14" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1141,6 +1171,9 @@
       <c r="AJ15" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="BB15" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1159,7 +1192,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>67</v>
       </c>
@@ -1173,7 +1206,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>68</v>
       </c>
@@ -1192,8 +1225,11 @@
       <c r="AM18" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="BB18" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>130</v>
       </c>
@@ -1207,7 +1243,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -1224,7 +1260,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -1237,8 +1273,11 @@
       <c r="AJ21" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="BB21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
@@ -1249,7 +1288,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
@@ -1260,7 +1299,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -1274,7 +1313,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -1288,7 +1327,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -1302,7 +1341,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -1310,7 +1349,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -1318,7 +1357,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
@@ -1332,7 +1371,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>79</v>
       </c>
@@ -1343,7 +1382,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
@@ -1354,7 +1393,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>81</v>
       </c>
@@ -1556,7 +1595,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
@@ -1570,7 +1609,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>99</v>
       </c>
@@ -1578,7 +1617,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>131</v>
       </c>
@@ -1588,8 +1627,11 @@
       <c r="AF51" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AO51" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>100</v>
       </c>
@@ -1600,7 +1642,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>132</v>
       </c>
@@ -1614,7 +1656,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>133</v>
       </c>
@@ -1625,7 +1667,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
@@ -1636,7 +1678,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -1644,358 +1686,604 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>103</v>
       </c>
       <c r="AB57" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AO57" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>104</v>
       </c>
       <c r="AB58" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AO58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ58" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB59" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP59" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="AB59" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="AB60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ60" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="AB60" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="AB61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ61" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AR62" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS62" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV62" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="AR63" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="AR64" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="65" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="AR65" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="65" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="AR66" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AR67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX67" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY67" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AR68" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW68" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR69" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV69" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX69" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AR70" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BA70" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AR71" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ71" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="66" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="BC72" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="67" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="BC73" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="68" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="BC74" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="76" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="70" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="AR76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AS76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AV76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BA76" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BB76" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM70" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="H77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM77" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT77" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="AB71" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ71" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK71" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL71" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM71" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="AB78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BB78" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC78" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="M72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="T72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="U72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AL72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AM72" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="M79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL79" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO79" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="M73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="T73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="U73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V73" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="M80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U80" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V80" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="M74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB74" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="M81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BB81" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="M75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="S75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="T75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="U75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="V75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE75" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="76" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="M82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="P82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="T82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BB82" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="AB76" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC76" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD76" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE76" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="77" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="AB83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO83" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="X77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB77" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="B84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB84" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="AB78" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="79" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="AB85" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC85" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="AB79" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC79" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ79" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="80" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="AB86" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC86" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ86" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>127</v>
+      </c>
+      <c r="AB87" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP88" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ88" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR89" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>